<commit_message>
toString for DataModel is added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Validate_Function_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Validate_Function_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="555" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,28 +61,28 @@
     <t>Text</t>
   </si>
   <si>
-    <t>Error</t>
-  </si>
-  <si>
-    <t>Warning</t>
-  </si>
-  <si>
     <t>Message A10</t>
   </si>
   <si>
     <t>-</t>
   </si>
   <si>
-    <t>Message A10, Error, C10, #VALUE!, #VALUE!</t>
-  </si>
-  <si>
-    <t>Message A2, Error, C2, 1.0, 1.0</t>
-  </si>
-  <si>
-    <t>Message A5, Warning, C5, true, true</t>
-  </si>
-  <si>
-    <t>Message A6, Error, C6, =IF(0=10,TRUE,FALSE), false</t>
+    <t>E</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Message A2, E, C2, 1.0, 1.0</t>
+  </si>
+  <si>
+    <t>Message A5, W, C5, true, true</t>
+  </si>
+  <si>
+    <t>Message A6, E, C6, =IF(0=10,TRUE,FALSE), false</t>
+  </si>
+  <si>
+    <t>Message A10, E, C10, #VALUE!, #VALUE!</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,19 +464,19 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="e">
-        <f ca="1">VALIDATE(1=2, "Message A2", C2, "Error")</f>
+        <f ca="1">VALIDATE(1=2, "Message A2", C2, "E")</f>
         <v>#NAME?</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
-        <f ca="1">VALIDATE(1&lt;&gt;2, B3, C3, "Warning")</f>
+        <f ca="1">VALIDATE(1&lt;&gt;2, B3, C3, "W")</f>
         <v>#NAME?</v>
       </c>
       <c r="B3" t="s">
@@ -486,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -501,10 +501,10 @@
         <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -519,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -528,7 +528,7 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -544,14 +544,14 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" t="b">
         <f>IF(0=10,TRUE,FALSE)</f>
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -567,10 +567,10 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
         <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -585,10 +585,10 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -603,10 +603,10 @@
         <v>-0.6</v>
       </c>
       <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" t="s">
         <v>16</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -615,19 +615,19 @@
         <v>#NAME?</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="e">
         <v>#VALUE!</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SO exception is fixed in SpreadsheetEvaluator
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Validate_Function_Test.xlsx
+++ b/calculation-engine/engine-tests/engine-it/src/test/resources/datamodel/Validate_Function_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1905" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -79,10 +79,10 @@
     <t>Message A5, W, C5, true, true</t>
   </si>
   <si>
-    <t>Message A6, E, C6, =IF(0=10,TRUE,FALSE), false</t>
-  </si>
-  <si>
     <t>Message A10, E, C10, #VALUE!, #VALUE!</t>
+  </si>
+  <si>
+    <t>Message A6, E, C6, IF(0=10,TRUE,FALSE), false</t>
   </si>
 </sst>
 </file>
@@ -428,7 +428,7 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +551,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -627,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="G10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>